<commit_message>
Features: Correción de fechas
Se modificaron los parámetros de fechas en las consultas de citas.
Se limita función de registro de prescripción sólo a empleados con posición "Doctor"
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/prescription.xlsx
+++ b/src/main/resources/templates/prescription.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\scimec\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70489E73-AD0F-4280-8285-140C63C4AD47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1C040D-8B3A-4D79-B5D4-FFC3B74F7A6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BC44764A-1076-4560-90F1-04A26E8447CE}"/>
   </bookViews>
@@ -37,9 +37,6 @@
     <t>Av. Universidad Tecnológica 1, Palo Escrito, 62765 Emiliano Zapata, Mor.</t>
   </si>
   <si>
-    <t>Medico General</t>
-  </si>
-  <si>
     <t>&lt;&lt;Nombre del médico&gt;&gt;</t>
   </si>
   <si>
@@ -74,6 +71,9 @@
   </si>
   <si>
     <t>Firma del paciente</t>
+  </si>
+  <si>
+    <t>Médico General</t>
   </si>
 </sst>
 </file>
@@ -194,41 +194,41 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -552,7 +552,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E848D7BD-55E0-4AF1-A6CE-193F990D3C46}">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
       <selection activeCell="A13" sqref="A13:I31"/>
     </sheetView>
   </sheetViews>
@@ -563,98 +563,98 @@
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+    </row>
+    <row r="3" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-    </row>
-    <row r="3" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
       <c r="H5" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I5" s="4"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
+        <v>4</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
       <c r="D7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="B9" s="12"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="17"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -664,8 +664,8 @@
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -884,10 +884,10 @@
       <c r="I31" s="15"/>
     </row>
     <row r="32" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B32" s="7"/>
+      <c r="A32" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="16"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
@@ -960,46 +960,46 @@
       <c r="H39" s="4"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B40" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="F40" s="8" t="s">
+      <c r="B40" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="F40" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G40" s="17"/>
+      <c r="H40" s="17"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
-      <c r="H43" s="6"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A11:B12"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="C9:G9"/>
     <mergeCell ref="B43:H43"/>
     <mergeCell ref="A13:I31"/>
     <mergeCell ref="A33:I37"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="F40:H40"/>
     <mergeCell ref="B40:D40"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A11:B12"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B7:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>